<commit_message>
analisa per cabang p.1
</commit_message>
<xml_diff>
--- a/Laporan_Benchmark_BBM.xlsx
+++ b/Laporan_Benchmark_BBM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD74A633-1730-46AE-8658-A4497FBDC67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB2E3CF-C6C9-43D5-8E32-884990C0A68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1249,12 +1249,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>17.75</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>78.61</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2294,7 @@
         <v>164.22</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2327,7 +2326,7 @@
         <v>193.32</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>217.35</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2391,7 +2390,7 @@
         <v>217.89</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2423,7 +2422,7 @@
         <v>292.64</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2455,7 +2454,7 @@
         <v>341.31</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2487,7 +2486,7 @@
         <v>462.15</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2518,7 @@
         <v>490.77</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2551,7 +2550,7 @@
         <v>496.32</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>563.24</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>772.8</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>792.78</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2679,7 +2678,7 @@
         <v>974.75</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>1181.05</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2743,7 +2742,7 @@
         <v>1194.08</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>1214.08</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2807,7 +2806,7 @@
         <v>1241.31</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2839,7 +2838,7 @@
         <v>1467.7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2871,7 +2870,7 @@
         <v>2122.36</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2903,7 +2902,7 @@
         <v>2554.9299999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2935,7 +2934,7 @@
         <v>3456.39</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2967,7 +2966,7 @@
         <v>4520.1000000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>4642.5600000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3031,7 +3030,7 @@
         <v>4730.18</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -3159,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3191,7 +3190,7 @@
         <v>298.68</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -3255,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -4055,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>84</v>
       </c>
@@ -4087,7 +4086,7 @@
         <v>194.7</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -4119,7 +4118,7 @@
         <v>400.14</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>84</v>
       </c>
@@ -4151,7 +4150,7 @@
         <v>498.52</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>84</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>593.65</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>84</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>84</v>
       </c>
@@ -4247,7 +4246,7 @@
         <v>1193.19</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>84</v>
       </c>
@@ -4279,7 +4278,7 @@
         <v>1309.46</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>84</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>3294.7</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>84</v>
       </c>
@@ -4343,7 +4342,7 @@
         <v>3441.01</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>84</v>
       </c>
@@ -4375,7 +4374,7 @@
         <v>5129.46</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>84</v>
       </c>
@@ -4407,7 +4406,7 @@
         <v>5215.79</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>84</v>
       </c>
@@ -4439,7 +4438,7 @@
         <v>5282.94</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>84</v>
       </c>
@@ -4471,7 +4470,7 @@
         <v>6349.2</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>84</v>
       </c>
@@ -4503,7 +4502,7 @@
         <v>6547.48</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>84</v>
       </c>
@@ -4535,7 +4534,7 @@
         <v>7824.6</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>84</v>
       </c>
@@ -4567,7 +4566,7 @@
         <v>9328.2199999999993</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>84</v>
       </c>
@@ -4599,7 +4598,7 @@
         <v>10047.07</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>84</v>
       </c>
@@ -4631,7 +4630,7 @@
         <v>10583.37</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>84</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>10587.03</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>84</v>
       </c>
@@ -4695,7 +4694,7 @@
         <v>11734.56</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>84</v>
       </c>
@@ -4727,7 +4726,7 @@
         <v>12155.52</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>84</v>
       </c>
@@ -4759,7 +4758,7 @@
         <v>13674.24</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>84</v>
       </c>
@@ -4791,7 +4790,7 @@
         <v>18562.740000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>84</v>
       </c>
@@ -5879,7 +5878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>134</v>
       </c>
@@ -5911,7 +5910,7 @@
         <v>31.75</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>134</v>
       </c>
@@ -5943,7 +5942,7 @@
         <v>205.5</v>
       </c>
     </row>
-    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>134</v>
       </c>
@@ -5975,7 +5974,7 @@
         <v>268.94</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>134</v>
       </c>
@@ -6007,7 +6006,7 @@
         <v>317.33999999999997</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>134</v>
       </c>
@@ -6039,7 +6038,7 @@
         <v>531.6</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>134</v>
       </c>
@@ -6071,7 +6070,7 @@
         <v>548.86</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>134</v>
       </c>
@@ -6103,7 +6102,7 @@
         <v>622.35</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>134</v>
       </c>
@@ -6135,7 +6134,7 @@
         <v>805.6</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>134</v>
       </c>
@@ -6167,7 +6166,7 @@
         <v>1022.34</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>134</v>
       </c>
@@ -6199,7 +6198,7 @@
         <v>1044.58</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>134</v>
       </c>
@@ -6231,7 +6230,7 @@
         <v>1101.2</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>134</v>
       </c>
@@ -6263,7 +6262,7 @@
         <v>2216.64</v>
       </c>
     </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>134</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>2274.23</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>134</v>
       </c>
@@ -6327,7 +6326,7 @@
         <v>2399.56</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>134</v>
       </c>
@@ -6359,7 +6358,7 @@
         <v>4867.5200000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>134</v>
       </c>
@@ -6391,7 +6390,7 @@
         <v>5845.67</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>134</v>
       </c>
@@ -6423,7 +6422,7 @@
         <v>5945.58</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>134</v>
       </c>
@@ -6455,7 +6454,7 @@
         <v>6001.6</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>134</v>
       </c>
@@ -6487,7 +6486,7 @@
         <v>6046.56</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>134</v>
       </c>
@@ -6519,7 +6518,7 @@
         <v>6106</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>134</v>
       </c>
@@ -6551,7 +6550,7 @@
         <v>6918.17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>134</v>
       </c>
@@ -6583,7 +6582,7 @@
         <v>7140</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>134</v>
       </c>
@@ -6615,7 +6614,7 @@
         <v>7310</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>134</v>
       </c>
@@ -6647,7 +6646,7 @@
         <v>7584.16</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>134</v>
       </c>
@@ -6679,7 +6678,7 @@
         <v>7874.93</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>134</v>
       </c>
@@ -6711,7 +6710,7 @@
         <v>8008.2</v>
       </c>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>134</v>
       </c>
@@ -6743,7 +6742,7 @@
         <v>9112</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>134</v>
       </c>
@@ -6775,7 +6774,7 @@
         <v>9145.68</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>134</v>
       </c>
@@ -6807,7 +6806,7 @@
         <v>9151.7000000000007</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>134</v>
       </c>
@@ -6839,7 +6838,7 @@
         <v>9496.2000000000007</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>134</v>
       </c>
@@ -6871,7 +6870,7 @@
         <v>9544.2800000000007</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>134</v>
       </c>
@@ -7191,7 +7190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>264</v>
       </c>
@@ -7223,7 +7222,7 @@
         <v>120.98</v>
       </c>
     </row>
-    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>264</v>
       </c>
@@ -7255,7 +7254,7 @@
         <v>421.84</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>264</v>
       </c>
@@ -7287,7 +7286,7 @@
         <v>1186.68</v>
       </c>
     </row>
-    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>264</v>
       </c>
@@ -7319,7 +7318,7 @@
         <v>1341.61</v>
       </c>
     </row>
-    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>264</v>
       </c>
@@ -7351,7 +7350,7 @@
         <v>3030.96</v>
       </c>
     </row>
-    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>264</v>
       </c>
@@ -7383,7 +7382,7 @@
         <v>3340.26</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>264</v>
       </c>
@@ -7415,7 +7414,7 @@
         <v>5975.28</v>
       </c>
     </row>
-    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>264</v>
       </c>
@@ -7449,11 +7448,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J193" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="EFISIEN (Hijau)"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J193">
       <sortCondition ref="C1:C193"/>
     </sortState>

</xml_diff>

<commit_message>
analisa per cabang dan per jenis alat berat
</commit_message>
<xml_diff>
--- a/Laporan_Benchmark_BBM.xlsx
+++ b/Laporan_Benchmark_BBM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB2E3CF-C6C9-43D5-8E32-884990C0A68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F096E0EB-9D4C-4DAE-9319-1E0213C29550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1252,8 +1252,8 @@
   <dimension ref="A1:J193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>